<commit_message>
:sparkles: feat: Add match result
</commit_message>
<xml_diff>
--- a/data/DadosCopaDoMundoQatar2022.xlsx
+++ b/data/DadosCopaDoMundoQatar2022.xlsx
@@ -1171,7 +1171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -1253,7 +1253,7 @@
         <v>1090</v>
       </c>
       <c r="G2" s="11">
-        <v>2252</v>
+        <v>2290</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>18</v>
@@ -1276,84 +1276,84 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E3" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11">
-        <v>559</v>
+        <v>886</v>
       </c>
       <c r="G3" s="11">
-        <v>1970</v>
+        <v>2064</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4" s="11">
-        <v>886</v>
+        <v>805</v>
       </c>
       <c r="G4" s="11">
-        <v>2064</v>
+        <v>2014</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1376,7 +1376,7 @@
         <v>1360</v>
       </c>
       <c r="G5" s="11">
-        <v>1981</v>
+        <v>2011</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>23</v>
@@ -1417,7 +1417,7 @@
         <v>608</v>
       </c>
       <c r="G6" s="11">
-        <v>2114</v>
+        <v>1971</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>18</v>
@@ -1440,43 +1440,43 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="11" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" s="11">
-        <v>805</v>
+        <v>559</v>
       </c>
       <c r="G7" s="11">
-        <v>1984</v>
+        <v>1958</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1540,7 +1540,7 @@
         <v>882</v>
       </c>
       <c r="G9" s="11">
-        <v>1868</v>
+        <v>1871</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>23</v>
@@ -1563,66 +1563,66 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="11" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10" s="11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F10" s="11">
-        <v>339.3</v>
+        <v>746.5</v>
       </c>
       <c r="G10" s="11">
-        <v>1810</v>
+        <v>1839</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="11">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F11" s="11">
-        <v>192.2</v>
+        <v>339.3</v>
       </c>
       <c r="G11" s="11">
-        <v>1687</v>
+        <v>1780</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>23</v>
@@ -1631,162 +1631,162 @@
         <v>0</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>182</v>
+        <v>115</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="11" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E12" s="11">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F12" s="11">
-        <v>369.4</v>
+        <v>395.4</v>
       </c>
       <c r="G12" s="11">
-        <v>1721</v>
+        <v>1748</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I12" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="11" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="11">
         <v>15</v>
       </c>
-      <c r="E13" s="11">
-        <v>12</v>
-      </c>
       <c r="F13" s="11">
-        <v>201.3</v>
+        <v>369.4</v>
       </c>
       <c r="G13" s="11">
-        <v>1633</v>
+        <v>1704</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I13" s="11">
         <v>0</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="11" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E14" s="11">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F14" s="11">
-        <v>395.4</v>
+        <v>192.2</v>
       </c>
       <c r="G14" s="11">
-        <v>1756</v>
+        <v>1692</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I14" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="E15" s="11">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" s="11">
-        <v>204.4</v>
+        <v>201.3</v>
       </c>
       <c r="G15" s="11">
-        <v>1620</v>
+        <v>1671</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>13</v>
@@ -1795,180 +1795,180 @@
         <v>0</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="11" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>127</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E16" s="11">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F16" s="11">
-        <v>746.5</v>
+        <v>131.69999999999999</v>
       </c>
       <c r="G16" s="11">
-        <v>1871</v>
+        <v>1639</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="I16" s="11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="11" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>127</v>
+        <v>168</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E17" s="11">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="11">
-        <v>131.69999999999999</v>
+        <v>328</v>
       </c>
       <c r="G17" s="11">
-        <v>1572</v>
+        <v>1622</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="I17" s="11">
         <v>0</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E18" s="11">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F18" s="11">
-        <v>130.85</v>
+        <v>204.4</v>
       </c>
       <c r="G18" s="11">
-        <v>1578</v>
+        <v>1620</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I18" s="11">
         <v>0</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="11" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>147</v>
+        <v>64</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>158</v>
+        <v>81</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E19" s="11">
+        <v>19</v>
+      </c>
+      <c r="F19" s="11">
+        <v>130.85</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1578</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F19" s="11">
-        <v>231.9</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1568</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="I19" s="11">
         <v>0</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>159</v>
+        <v>82</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>160</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1991,7 +1991,7 @@
         <v>286.5</v>
       </c>
       <c r="G20" s="11">
-        <v>1602</v>
+        <v>1576</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>7</v>
@@ -2055,66 +2055,66 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="11" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E22" s="11">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" s="11">
-        <v>328</v>
+        <v>231.9</v>
       </c>
       <c r="G22" s="11">
-        <v>1642</v>
+        <v>1568</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="I22" s="11">
         <v>0</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="11" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" s="11">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="F23" s="11">
-        <v>68.58</v>
+        <v>23.1</v>
       </c>
       <c r="G23" s="11">
-        <v>1578</v>
+        <v>1563</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>1</v>
@@ -2123,39 +2123,39 @@
         <v>0</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="11" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>188</v>
+        <v>64</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>204</v>
+        <v>70</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" s="11">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F24" s="11">
-        <v>159.55000000000001</v>
+        <v>68.58</v>
       </c>
       <c r="G24" s="11">
-        <v>1550</v>
+        <v>1558</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>1</v>
@@ -2164,262 +2164,262 @@
         <v>0</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>207</v>
+        <v>73</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>205</v>
+        <v>71</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>206</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="11" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E25" s="11">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F25" s="11">
-        <v>65.849999999999994</v>
+        <v>125.8</v>
       </c>
       <c r="G25" s="11">
-        <v>1518</v>
+        <v>1552</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I25" s="11">
         <v>0</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="M25" s="11" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="11" t="s">
-        <v>16</v>
+        <v>203</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26" s="11">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F26" s="11">
-        <v>11.95</v>
+        <v>159.55000000000001</v>
       </c>
       <c r="G26" s="11">
-        <v>1523</v>
+        <v>1550</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I26" s="11">
         <v>0</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>145</v>
+        <v>207</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="11" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E27" s="11">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F27" s="11">
-        <v>125.8</v>
+        <v>11.95</v>
       </c>
       <c r="G27" s="11">
-        <v>1517</v>
+        <v>1523</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I27" s="11">
         <v>0</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="11" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E28" s="11">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="F28" s="11">
-        <v>23.1</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="G28" s="11">
-        <v>1463</v>
+        <v>1518</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I28" s="11">
         <v>0</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="11" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E29" s="11">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F29" s="11">
-        <v>40.33</v>
+        <v>172.13</v>
       </c>
       <c r="G29" s="11">
-        <v>1511</v>
+        <v>1513</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I29" s="11">
         <v>0</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="11" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E30" s="11">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F30" s="11">
-        <v>172.13</v>
+        <v>40.33</v>
       </c>
       <c r="G30" s="11">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I30" s="11">
         <v>0</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2554,100 +2554,100 @@
   <hyperlinks>
     <hyperlink ref="L32" r:id="rId1"/>
     <hyperlink ref="M32" r:id="rId2"/>
-    <hyperlink ref="L27" r:id="rId3"/>
-    <hyperlink ref="M27" r:id="rId4"/>
+    <hyperlink ref="L25" r:id="rId3"/>
+    <hyperlink ref="M25" r:id="rId4"/>
     <hyperlink ref="L20" r:id="rId5"/>
     <hyperlink ref="M20" r:id="rId6"/>
     <hyperlink ref="L8" r:id="rId7"/>
     <hyperlink ref="M8" r:id="rId8"/>
     <hyperlink ref="L5" r:id="rId9"/>
     <hyperlink ref="M5" r:id="rId10"/>
-    <hyperlink ref="L23" r:id="rId11"/>
-    <hyperlink ref="M23" r:id="rId12"/>
-    <hyperlink ref="L15" r:id="rId13"/>
-    <hyperlink ref="M15" r:id="rId14"/>
-    <hyperlink ref="L18" r:id="rId15"/>
-    <hyperlink ref="M18" r:id="rId16"/>
+    <hyperlink ref="L24" r:id="rId11"/>
+    <hyperlink ref="M24" r:id="rId12"/>
+    <hyperlink ref="L18" r:id="rId13"/>
+    <hyperlink ref="M18" r:id="rId14"/>
+    <hyperlink ref="L19" r:id="rId15"/>
+    <hyperlink ref="M19" r:id="rId16"/>
     <hyperlink ref="L6" r:id="rId17"/>
     <hyperlink ref="M6" r:id="rId18"/>
-    <hyperlink ref="L28" r:id="rId19"/>
-    <hyperlink ref="M28" r:id="rId20"/>
-    <hyperlink ref="L13" r:id="rId21"/>
-    <hyperlink ref="M13" r:id="rId22"/>
+    <hyperlink ref="L23" r:id="rId19"/>
+    <hyperlink ref="M23" r:id="rId20"/>
+    <hyperlink ref="L15" r:id="rId21"/>
+    <hyperlink ref="M15" r:id="rId22"/>
     <hyperlink ref="L21" r:id="rId23"/>
     <hyperlink ref="M21" r:id="rId24"/>
-    <hyperlink ref="L4" r:id="rId25"/>
-    <hyperlink ref="M4" r:id="rId26"/>
-    <hyperlink ref="L10" r:id="rId27"/>
-    <hyperlink ref="M10" r:id="rId28"/>
-    <hyperlink ref="L25" r:id="rId29"/>
-    <hyperlink ref="M25" r:id="rId30"/>
-    <hyperlink ref="L29" r:id="rId31"/>
-    <hyperlink ref="M29" r:id="rId32"/>
-    <hyperlink ref="L7" r:id="rId33"/>
-    <hyperlink ref="M7" r:id="rId34"/>
-    <hyperlink ref="L16" r:id="rId35"/>
-    <hyperlink ref="M16" r:id="rId36"/>
-    <hyperlink ref="L17" r:id="rId37"/>
-    <hyperlink ref="M17" r:id="rId38"/>
-    <hyperlink ref="L26" r:id="rId39"/>
-    <hyperlink ref="M26" r:id="rId40"/>
-    <hyperlink ref="L3" r:id="rId41"/>
-    <hyperlink ref="M3" r:id="rId42"/>
-    <hyperlink ref="L30" r:id="rId43"/>
-    <hyperlink ref="M30" r:id="rId44"/>
-    <hyperlink ref="L19" r:id="rId45"/>
-    <hyperlink ref="M19" r:id="rId46"/>
-    <hyperlink ref="L12" r:id="rId47"/>
-    <hyperlink ref="M12" r:id="rId48"/>
+    <hyperlink ref="L3" r:id="rId25"/>
+    <hyperlink ref="M3" r:id="rId26"/>
+    <hyperlink ref="L11" r:id="rId27"/>
+    <hyperlink ref="M11" r:id="rId28"/>
+    <hyperlink ref="L28" r:id="rId29"/>
+    <hyperlink ref="M28" r:id="rId30"/>
+    <hyperlink ref="L30" r:id="rId31"/>
+    <hyperlink ref="M30" r:id="rId32"/>
+    <hyperlink ref="L4" r:id="rId33"/>
+    <hyperlink ref="M4" r:id="rId34"/>
+    <hyperlink ref="L10" r:id="rId35"/>
+    <hyperlink ref="M10" r:id="rId36"/>
+    <hyperlink ref="L16" r:id="rId37"/>
+    <hyperlink ref="M16" r:id="rId38"/>
+    <hyperlink ref="L27" r:id="rId39"/>
+    <hyperlink ref="M27" r:id="rId40"/>
+    <hyperlink ref="L7" r:id="rId41"/>
+    <hyperlink ref="M7" r:id="rId42"/>
+    <hyperlink ref="L29" r:id="rId43"/>
+    <hyperlink ref="M29" r:id="rId44"/>
+    <hyperlink ref="L22" r:id="rId45"/>
+    <hyperlink ref="M22" r:id="rId46"/>
+    <hyperlink ref="L13" r:id="rId47"/>
+    <hyperlink ref="M13" r:id="rId48"/>
     <hyperlink ref="L2" r:id="rId49"/>
     <hyperlink ref="M2" r:id="rId50"/>
-    <hyperlink ref="L22" r:id="rId51"/>
-    <hyperlink ref="M22" r:id="rId52"/>
-    <hyperlink ref="L11" r:id="rId53"/>
-    <hyperlink ref="M11" r:id="rId54"/>
+    <hyperlink ref="L17" r:id="rId51"/>
+    <hyperlink ref="M17" r:id="rId52"/>
+    <hyperlink ref="L14" r:id="rId53"/>
+    <hyperlink ref="M14" r:id="rId54"/>
     <hyperlink ref="L31" r:id="rId55"/>
     <hyperlink ref="M31" r:id="rId56"/>
     <hyperlink ref="L9" r:id="rId57"/>
     <hyperlink ref="M9" r:id="rId58"/>
     <hyperlink ref="L33" r:id="rId59"/>
     <hyperlink ref="M33" r:id="rId60"/>
-    <hyperlink ref="L14" r:id="rId61"/>
-    <hyperlink ref="M14" r:id="rId62"/>
-    <hyperlink ref="L24" r:id="rId63"/>
-    <hyperlink ref="M24" r:id="rId64"/>
+    <hyperlink ref="L12" r:id="rId61"/>
+    <hyperlink ref="M12" r:id="rId62"/>
+    <hyperlink ref="L26" r:id="rId63"/>
+    <hyperlink ref="M26" r:id="rId64"/>
     <hyperlink ref="K6" r:id="rId65"/>
-    <hyperlink ref="K29" r:id="rId66" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K3" r:id="rId67" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K30" r:id="rId66" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K7" r:id="rId67" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K2" r:id="rId68" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K31" r:id="rId69" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K30" r:id="rId70" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K26" r:id="rId71" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K12" r:id="rId72" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K10" r:id="rId73" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K27" r:id="rId74" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K29" r:id="rId70" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K27" r:id="rId71" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K13" r:id="rId72" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K11" r:id="rId73" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K25" r:id="rId74" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K5" r:id="rId75" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K4" r:id="rId76" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K16" r:id="rId77" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K3" r:id="rId76" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K10" r:id="rId77" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K33" r:id="rId78" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K23" r:id="rId79" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K17" r:id="rId80" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K13" r:id="rId81" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K19" r:id="rId82" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K24" r:id="rId79" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K16" r:id="rId80" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K15" r:id="rId81" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K22" r:id="rId82" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K8" r:id="rId83" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K21" r:id="rId84" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K9" r:id="rId85" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K32" r:id="rId86" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K28" r:id="rId87" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K23" r:id="rId87" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
     <hyperlink ref="K20" r:id="rId88" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K22" r:id="rId89" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K24" r:id="rId90" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K7" r:id="rId91" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K11" r:id="rId92" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K25" r:id="rId93" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K15" r:id="rId94" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K14" r:id="rId95" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K18" r:id="rId96" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K17" r:id="rId89" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K26" r:id="rId90" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K4" r:id="rId91" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K14" r:id="rId92" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K28" r:id="rId93" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K18" r:id="rId94" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K12" r:id="rId95" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="K19" r:id="rId96" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId97"/>

</xml_diff>

<commit_message>
:sparkles: feat: New equationto avg goals and data update
</commit_message>
<xml_diff>
--- a/data/DadosCopaDoMundoQatar2022.xlsx
+++ b/data/DadosCopaDoMundoQatar2022.xlsx
@@ -16,7 +16,7 @@
     <sheet name="jogos" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">selecoes!$A$1:$M$1000</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">selecoes!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="156">
   <si>
     <t>South Korea</t>
   </si>
   <si>
-    <t>AFC</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Qatar</t>
   </si>
   <si>
-    <t>CAF</t>
-  </si>
-  <si>
     <t>Senegal</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Tunisia</t>
   </si>
   <si>
-    <t>CONCACAF</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>CONMEBOL</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>England</t>
   </si>
   <si>
-    <t>UEFA</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
@@ -155,28 +140,181 @@
     <t>Grupo</t>
   </si>
   <si>
-    <t>GrupoNumero</t>
-  </si>
-  <si>
     <t>NomeEmIngles</t>
   </si>
   <si>
-    <t>Copas</t>
-  </si>
-  <si>
-    <t>JogadorDestaque</t>
-  </si>
-  <si>
-    <t>FotoJogadorDestaque</t>
-  </si>
-  <si>
     <t>Catar</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>A1</t>
+    <t>Equador</t>
+  </si>
+  <si>
+    <t>Holanda</t>
+  </si>
+  <si>
+    <t>Inglaterra</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Irã</t>
+  </si>
+  <si>
+    <t>Estados Unidos</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>País de Gales</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Arábia Saudita</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Polônia</t>
+  </si>
+  <si>
+    <t>França</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Dinamarca</t>
+  </si>
+  <si>
+    <t>Tunísia</t>
+  </si>
+  <si>
+    <t>Austrália</t>
+  </si>
+  <si>
+    <t>Espanha</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Alemanha</t>
+  </si>
+  <si>
+    <t>Japão</t>
+  </si>
+  <si>
+    <t>Bélgica</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Canadá</t>
+  </si>
+  <si>
+    <t>Marrocos</t>
+  </si>
+  <si>
+    <t>Croácia</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Sérvia</t>
+  </si>
+  <si>
+    <t>Suíça</t>
+  </si>
+  <si>
+    <t>Camarões</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Gana</t>
+  </si>
+  <si>
+    <t>Uruguai</t>
+  </si>
+  <si>
+    <t>Coreia do Sul</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>seleção1</t>
+  </si>
+  <si>
+    <t>seleção2</t>
+  </si>
+  <si>
+    <t>estádio</t>
+  </si>
+  <si>
+    <t>AL THUMAMA</t>
+  </si>
+  <si>
+    <t>AL KHOR</t>
+  </si>
+  <si>
+    <t>INTER. KHALIFA</t>
+  </si>
+  <si>
+    <t>AL RAYYAN</t>
+  </si>
+  <si>
+    <t>CID. EDUCAÇÃO</t>
+  </si>
+  <si>
+    <t>AL WAKRAH</t>
+  </si>
+  <si>
+    <t>NAC. DE LUSAIL</t>
+  </si>
+  <si>
+    <t>PORTO DE DOHA</t>
+  </si>
+  <si>
+    <t>INTE. KHALIFA</t>
+  </si>
+  <si>
+    <t>NAC. LUSAIL</t>
+  </si>
+  <si>
+    <t>PontosRankingFIFA</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>LinkBandeiraPequena</t>
+  </si>
+  <si>
+    <t>LinkBandeiraGrande</t>
   </si>
   <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/QAT?tx=c_fill,g_auto,q_auto</t>
@@ -185,646 +323,190 @@
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Qatar_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Almoez Ali</t>
-  </si>
-  <si>
-    <t>Equador</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/ECU?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Ecuador_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Pervis Estupiñán</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/SEN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Senegal_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Sadio Mané</t>
-  </si>
-  <si>
-    <t>Holanda</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/NED?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Netherlands_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Virgil Van Dijk</t>
-  </si>
-  <si>
-    <t>Inglaterra</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/ENG?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_England_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Harry Kane</t>
-  </si>
-  <si>
-    <t>Irã</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/IRN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Iran_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Sardar Azmoun</t>
-  </si>
-  <si>
-    <t>Estados Unidos</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/USA?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_United_States_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Christian Pulisic</t>
-  </si>
-  <si>
-    <t>País de Gales</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/WAL?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Wales_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Gareth Bale</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/ARG?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Argentina_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Lionel Messi</t>
-  </si>
-  <si>
-    <t>Arábia Saudita</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/KSA?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Saudi_Arabia_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Salem Al-Dawsari</t>
-  </si>
-  <si>
-    <t>México</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/MEX?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Mexico_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Raúl Jiménez</t>
-  </si>
-  <si>
-    <t>Polônia</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/POL?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Poland_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Robert Lewandowski</t>
-  </si>
-  <si>
-    <t>França</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/FRA?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_France_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Kylian Mbappé</t>
-  </si>
-  <si>
-    <t>Dinamarca</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/DEN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Denmark_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Christian Eriksen</t>
-  </si>
-  <si>
-    <t>Tunísia</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/TUN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Tunisia_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Wahbi Khazri</t>
-  </si>
-  <si>
-    <t>Austrália</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/AUS?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Australia_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Ajdin Hrustic</t>
-  </si>
-  <si>
-    <t>Espanha</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/ESP?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Spain_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Pedri</t>
-  </si>
-  <si>
-    <t>Alemanha</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/GER?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Germany_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Thomas Müller</t>
-  </si>
-  <si>
-    <t>Japão</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/JPN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Japan_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Takumi Minamino</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/CRC?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Costa_Rica_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Keylor Navas</t>
-  </si>
-  <si>
-    <t>Bélgica</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/BEL?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Belgium_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Kevin De Bruyne</t>
-  </si>
-  <si>
-    <t>Canadá</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/CAN?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Canada_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Alphonso Davies</t>
-  </si>
-  <si>
-    <t>Marrocos</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/MAR?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Morocco_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Achraf Hakimi</t>
-  </si>
-  <si>
-    <t>Croácia</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/CRO?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Croatia_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Luka Modric</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/BRA?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Brazil_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Neymar Jr.</t>
-  </si>
-  <si>
-    <t>Sérvia</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/SRB?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Serbia_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Dusan Vlahovic</t>
-  </si>
-  <si>
-    <t>Suíça</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/SUI?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Switzerland_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Granit Xhaka</t>
-  </si>
-  <si>
-    <t>Camarões</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/CMR?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Cameroon_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Frank Anguissa</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/POR?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Portugal_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Cristiano Ronaldo</t>
-  </si>
-  <si>
-    <t>Gana</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/GHA?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Ghana_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Thomas Partey</t>
-  </si>
-  <si>
-    <t>Uruguai</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/URU?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_Uruguay_Flat_Round_Corner-512x512.png</t>
   </si>
   <si>
-    <t>Federico Valverde</t>
-  </si>
-  <si>
-    <t>Coreia do Sul</t>
-  </si>
-  <si>
-    <t>H4</t>
-  </si>
-  <si>
     <t>https://cloudinary.fifa.com/api/v3/picture/flags-sq-2/KOR?tx=c_fill,g_auto,q_auto</t>
   </si>
   <si>
     <t>https://flagdownload.com/wp-content/uploads/Flag_of_South_Korea_Flat_Round_Corner-512x512.png</t>
-  </si>
-  <si>
-    <t>Heung-Min Son</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>hora</t>
-  </si>
-  <si>
-    <t>grupo</t>
-  </si>
-  <si>
-    <t>seleção1</t>
-  </si>
-  <si>
-    <t>seleção2</t>
-  </si>
-  <si>
-    <t>estádio</t>
-  </si>
-  <si>
-    <t>AL THUMAMA</t>
-  </si>
-  <si>
-    <t>AL KHOR</t>
-  </si>
-  <si>
-    <t>INTER. KHALIFA</t>
-  </si>
-  <si>
-    <t>AL RAYYAN</t>
-  </si>
-  <si>
-    <t>CID. EDUCAÇÃO</t>
-  </si>
-  <si>
-    <t>AL WAKRAH</t>
-  </si>
-  <si>
-    <t>NAC. DE LUSAIL</t>
-  </si>
-  <si>
-    <t>PORTO DE DOHA</t>
-  </si>
-  <si>
-    <t>INTE. KHALIFA</t>
-  </si>
-  <si>
-    <t>NAC. LUSAIL</t>
-  </si>
-  <si>
-    <t>LinkBandeiraGrande</t>
-  </si>
-  <si>
-    <t>LinkBandeiraPequena</t>
-  </si>
-  <si>
-    <t>PontosRankingFIFA</t>
-  </si>
-  <si>
-    <t>PosiçãoRankingFIFA</t>
-  </si>
-  <si>
-    <t>ValorDeMercado</t>
-  </si>
-  <si>
-    <t>Confederação</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide32.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide2.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide3.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide4.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide5.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide6.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide7.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide8.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide9.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide10.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide11.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide12.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide13.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide14.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide15.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide16.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide17.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide18.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide19.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide20.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide21.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide22.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide23.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide24.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide25.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide26.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide27.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide28.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide29.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide30.JPG?raw=true</t>
-  </si>
-  <si>
-    <t>https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide31.JPG?raw=true</t>
   </si>
 </sst>
 </file>
@@ -834,7 +516,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,6 +581,13 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -920,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,6 +643,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,1488 +860,965 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="25.85546875" style="11" customWidth="1"/>
-    <col min="14" max="18" width="8.7109375" style="11" customWidth="1"/>
-    <col min="19" max="16384" width="14.42578125" style="11"/>
+    <col min="3" max="3" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="72.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="95.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" spans="1:8" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="13">
+        <v>88.9</v>
+      </c>
+      <c r="E2" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="13">
+        <v>62</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="13">
+        <v>86</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13">
+        <v>62.4</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="13">
+        <v>93.5</v>
+      </c>
+      <c r="E7" s="11">
+        <v>3.1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13">
+        <v>64.5</v>
+      </c>
+      <c r="E8" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="13">
+        <v>71.5</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>48.5</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <v>70.3</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="13">
+        <v>52.9</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="13">
+        <v>77.7</v>
+      </c>
+      <c r="E14" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="13">
+        <v>75.8</v>
+      </c>
+      <c r="E15" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="13">
+        <v>90.6</v>
+      </c>
+      <c r="E16" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="13">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="13">
+        <v>90.1</v>
+      </c>
+      <c r="E18" s="11">
+        <v>3</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="13">
+        <v>60.5</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="B20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="13">
+        <v>84.4</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2.6</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="C21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="13">
+        <v>85.4</v>
+      </c>
+      <c r="E21" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="B22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="13">
+        <v>69.3</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="11">
-        <v>1090</v>
-      </c>
-      <c r="G2" s="11">
-        <v>2290</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="11">
-        <v>5</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="11">
-        <v>4</v>
-      </c>
-      <c r="F3" s="11">
-        <v>886</v>
-      </c>
-      <c r="G3" s="11">
-        <v>2064</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="11">
+      <c r="D23" s="13">
+        <v>73.7</v>
+      </c>
+      <c r="E23" s="11">
         <v>2</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="F23" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="11">
-        <v>6</v>
-      </c>
-      <c r="F4" s="11">
-        <v>805</v>
-      </c>
-      <c r="G4" s="11">
-        <v>2014</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="11">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="L4" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="11">
-        <v>5</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1360</v>
-      </c>
-      <c r="G5" s="11">
-        <v>2011</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="11">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="11">
-        <v>3</v>
-      </c>
-      <c r="F6" s="11">
-        <v>608</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1971</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="11">
-        <v>2</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="11">
-        <v>2</v>
-      </c>
-      <c r="F7" s="11">
-        <v>559</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1958</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="11">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="11" t="s">
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="11">
-        <v>8</v>
-      </c>
-      <c r="F8" s="11">
-        <v>455.75</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1900</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="11">
-        <v>9</v>
-      </c>
-      <c r="F9" s="11">
-        <v>882</v>
-      </c>
-      <c r="G9" s="11">
-        <v>1871</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="11">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="11">
-        <v>11</v>
-      </c>
-      <c r="F10" s="11">
-        <v>746.5</v>
-      </c>
-      <c r="G10" s="11">
-        <v>1839</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="11">
-        <v>4</v>
-      </c>
-      <c r="J10" s="11" t="s">
+      <c r="C24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="13">
+        <v>75</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="F24" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="11">
-        <v>339.3</v>
-      </c>
-      <c r="G11" s="11">
-        <v>1780</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="11">
-        <v>13</v>
-      </c>
-      <c r="F12" s="11">
-        <v>395.4</v>
-      </c>
-      <c r="G12" s="11">
-        <v>1748</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="11">
-        <v>2</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="11">
-        <v>15</v>
-      </c>
-      <c r="F13" s="11">
-        <v>369.4</v>
-      </c>
-      <c r="G13" s="11">
-        <v>1704</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="11">
-        <v>0</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="11">
-        <v>16</v>
-      </c>
-      <c r="F14" s="11">
-        <v>192.2</v>
-      </c>
-      <c r="G14" s="11">
-        <v>1692</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="11">
-        <v>0</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="11">
-        <v>12</v>
-      </c>
-      <c r="F15" s="11">
-        <v>201.3</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1671</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="11">
-        <v>0</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="11">
-        <v>24</v>
-      </c>
-      <c r="F16" s="11">
-        <v>131.69999999999999</v>
-      </c>
-      <c r="G16" s="11">
-        <v>1639</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="11">
-        <v>0</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="11">
-        <v>25</v>
-      </c>
-      <c r="F17" s="11">
-        <v>328</v>
-      </c>
-      <c r="G17" s="11">
-        <v>1622</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="11">
-        <v>0</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="11">
-        <v>14</v>
-      </c>
-      <c r="F18" s="11">
-        <v>204.4</v>
-      </c>
-      <c r="G18" s="11">
-        <v>1620</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="11">
-        <v>0</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="11">
-        <v>19</v>
-      </c>
-      <c r="F19" s="11">
-        <v>130.85</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1578</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="11">
-        <v>0</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="M19" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="11">
-        <v>18</v>
-      </c>
-      <c r="F20" s="11">
-        <v>286.5</v>
-      </c>
-      <c r="G20" s="11">
-        <v>1576</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M20" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="11">
-        <v>26</v>
-      </c>
-      <c r="F21" s="11">
-        <v>257.7</v>
-      </c>
-      <c r="G21" s="11">
-        <v>1569</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="11">
-        <v>0</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="M21" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="11">
-        <v>23</v>
-      </c>
-      <c r="F22" s="11">
-        <v>231.9</v>
-      </c>
-      <c r="G22" s="11">
-        <v>1568</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="11">
-        <v>0</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="M22" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="11">
-        <v>53</v>
-      </c>
-      <c r="F23" s="11">
-        <v>23.1</v>
-      </c>
-      <c r="G23" s="11">
-        <v>1563</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="11">
-        <v>0</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="L23" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="11">
-        <v>22</v>
-      </c>
-      <c r="F24" s="11">
-        <v>68.58</v>
-      </c>
-      <c r="G24" s="11">
-        <v>1558</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="11">
-        <v>0</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="L24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="D25" s="13">
+        <v>72.400000000000006</v>
       </c>
       <c r="E25" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="13">
+        <v>65.2</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="11">
-        <v>125.8</v>
-      </c>
-      <c r="G25" s="11">
-        <v>1552</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="11">
-        <v>0</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="L25" s="11" t="s">
+      <c r="C27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="13">
+        <v>69</v>
+      </c>
+      <c r="E27" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="13">
+        <v>87.6</v>
+      </c>
+      <c r="E28" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="13">
+        <v>73</v>
+      </c>
+      <c r="E29" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="F29" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="13">
+        <v>74.7</v>
+      </c>
+      <c r="E30" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F30" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="13">
+        <v>77</v>
+      </c>
+      <c r="E31" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="F31" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="M25" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11">
-        <v>28</v>
-      </c>
-      <c r="F26" s="11">
-        <v>159.55000000000001</v>
-      </c>
-      <c r="G26" s="11">
-        <v>1550</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="L26" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="M26" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="11" t="s">
+      <c r="B32" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="13">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="11">
-        <v>34</v>
-      </c>
-      <c r="F27" s="11">
-        <v>11.95</v>
-      </c>
-      <c r="G27" s="11">
-        <v>1523</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="11">
-        <v>0</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="L27" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="M27" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="11">
-        <v>30</v>
-      </c>
-      <c r="F28" s="11">
-        <v>65.849999999999994</v>
-      </c>
-      <c r="G28" s="11">
-        <v>1518</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="11">
-        <v>0</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="M28" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="11" t="s">
+      <c r="D33" s="13">
+        <v>79.3</v>
+      </c>
+      <c r="E33" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="F33" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="11" t="s">
+      <c r="H33" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="11">
-        <v>43</v>
-      </c>
-      <c r="F29" s="11">
-        <v>172.13</v>
-      </c>
-      <c r="G29" s="11">
-        <v>1513</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="11">
-        <v>0</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="L29" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="M29" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="11">
-        <v>39</v>
-      </c>
-      <c r="F30" s="11">
-        <v>40.33</v>
-      </c>
-      <c r="G30" s="11">
-        <v>1511</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="11">
-        <v>38</v>
-      </c>
-      <c r="F31" s="11">
-        <v>114.75</v>
-      </c>
-      <c r="G31" s="11">
-        <v>1483</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="L31" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="M31" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="11">
-        <v>48</v>
-      </c>
-      <c r="F32" s="11">
-        <v>18.329999999999998</v>
-      </c>
-      <c r="G32" s="11">
-        <v>1469</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="11">
-        <v>0</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="L32" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="11">
-        <v>60</v>
-      </c>
-      <c r="F33" s="11">
-        <v>206.4</v>
-      </c>
-      <c r="G33" s="11">
-        <v>1419</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="11">
-        <v>0</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="L33" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="M33" s="11" t="s">
-        <v>196</v>
-      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="H36" s="14"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="G44" s="14"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="H46" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1000">
-    <sortState ref="A2:M33">
-      <sortCondition descending="1" ref="G1:G1000"/>
+  <autoFilter ref="A1:H1">
+    <sortState ref="A2:H33">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="L32" r:id="rId1"/>
-    <hyperlink ref="M32" r:id="rId2"/>
-    <hyperlink ref="L25" r:id="rId3"/>
-    <hyperlink ref="M25" r:id="rId4"/>
-    <hyperlink ref="L20" r:id="rId5"/>
-    <hyperlink ref="M20" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="M8" r:id="rId8"/>
-    <hyperlink ref="L5" r:id="rId9"/>
-    <hyperlink ref="M5" r:id="rId10"/>
-    <hyperlink ref="L24" r:id="rId11"/>
-    <hyperlink ref="M24" r:id="rId12"/>
-    <hyperlink ref="L18" r:id="rId13"/>
-    <hyperlink ref="M18" r:id="rId14"/>
-    <hyperlink ref="L19" r:id="rId15"/>
-    <hyperlink ref="M19" r:id="rId16"/>
-    <hyperlink ref="L6" r:id="rId17"/>
-    <hyperlink ref="M6" r:id="rId18"/>
-    <hyperlink ref="L23" r:id="rId19"/>
-    <hyperlink ref="M23" r:id="rId20"/>
-    <hyperlink ref="L15" r:id="rId21"/>
-    <hyperlink ref="M15" r:id="rId22"/>
-    <hyperlink ref="L21" r:id="rId23"/>
-    <hyperlink ref="M21" r:id="rId24"/>
-    <hyperlink ref="L3" r:id="rId25"/>
-    <hyperlink ref="M3" r:id="rId26"/>
-    <hyperlink ref="L11" r:id="rId27"/>
-    <hyperlink ref="M11" r:id="rId28"/>
-    <hyperlink ref="L28" r:id="rId29"/>
-    <hyperlink ref="M28" r:id="rId30"/>
-    <hyperlink ref="L30" r:id="rId31"/>
-    <hyperlink ref="M30" r:id="rId32"/>
-    <hyperlink ref="L4" r:id="rId33"/>
-    <hyperlink ref="M4" r:id="rId34"/>
-    <hyperlink ref="L10" r:id="rId35"/>
-    <hyperlink ref="M10" r:id="rId36"/>
-    <hyperlink ref="L16" r:id="rId37"/>
-    <hyperlink ref="M16" r:id="rId38"/>
-    <hyperlink ref="L27" r:id="rId39"/>
-    <hyperlink ref="M27" r:id="rId40"/>
-    <hyperlink ref="L7" r:id="rId41"/>
-    <hyperlink ref="M7" r:id="rId42"/>
-    <hyperlink ref="L29" r:id="rId43"/>
-    <hyperlink ref="M29" r:id="rId44"/>
-    <hyperlink ref="L22" r:id="rId45"/>
-    <hyperlink ref="M22" r:id="rId46"/>
-    <hyperlink ref="L13" r:id="rId47"/>
-    <hyperlink ref="M13" r:id="rId48"/>
-    <hyperlink ref="L2" r:id="rId49"/>
-    <hyperlink ref="M2" r:id="rId50"/>
-    <hyperlink ref="L17" r:id="rId51"/>
-    <hyperlink ref="M17" r:id="rId52"/>
-    <hyperlink ref="L14" r:id="rId53"/>
-    <hyperlink ref="M14" r:id="rId54"/>
-    <hyperlink ref="L31" r:id="rId55"/>
-    <hyperlink ref="M31" r:id="rId56"/>
-    <hyperlink ref="L9" r:id="rId57"/>
-    <hyperlink ref="M9" r:id="rId58"/>
-    <hyperlink ref="L33" r:id="rId59"/>
-    <hyperlink ref="M33" r:id="rId60"/>
-    <hyperlink ref="L12" r:id="rId61"/>
-    <hyperlink ref="M12" r:id="rId62"/>
-    <hyperlink ref="L26" r:id="rId63"/>
-    <hyperlink ref="M26" r:id="rId64"/>
-    <hyperlink ref="K6" r:id="rId65"/>
-    <hyperlink ref="K30" r:id="rId66" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K7" r:id="rId67" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K2" r:id="rId68" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K31" r:id="rId69" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K29" r:id="rId70" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K27" r:id="rId71" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K13" r:id="rId72" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K11" r:id="rId73" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K25" r:id="rId74" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K5" r:id="rId75" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K3" r:id="rId76" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K10" r:id="rId77" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K33" r:id="rId78" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K24" r:id="rId79" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K16" r:id="rId80" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K15" r:id="rId81" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K22" r:id="rId82" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K8" r:id="rId83" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K21" r:id="rId84" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K9" r:id="rId85" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K32" r:id="rId86" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K23" r:id="rId87" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K20" r:id="rId88" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K17" r:id="rId89" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K26" r:id="rId90" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K4" r:id="rId91" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K14" r:id="rId92" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K28" r:id="rId93" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K18" r:id="rId94" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K12" r:id="rId95" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
-    <hyperlink ref="K19" r:id="rId96" display="https://github.com/ricardorocha86/PrevisaoEsportiva/blob/main/FotoJogadores/Slide1.JPG?raw=true"/>
+    <hyperlink ref="G10" r:id="rId1"/>
+    <hyperlink ref="H10" r:id="rId2"/>
+    <hyperlink ref="G15" r:id="rId3"/>
+    <hyperlink ref="H15" r:id="rId4"/>
+    <hyperlink ref="G29" r:id="rId5"/>
+    <hyperlink ref="H29" r:id="rId6"/>
+    <hyperlink ref="G20" r:id="rId7"/>
+    <hyperlink ref="H20" r:id="rId8"/>
+    <hyperlink ref="G21" r:id="rId9"/>
+    <hyperlink ref="H21" r:id="rId10"/>
+    <hyperlink ref="G22" r:id="rId11"/>
+    <hyperlink ref="H22" r:id="rId12"/>
+    <hyperlink ref="G17" r:id="rId13"/>
+    <hyperlink ref="H17" r:id="rId14"/>
+    <hyperlink ref="G26" r:id="rId15"/>
+    <hyperlink ref="H26" r:id="rId16"/>
+    <hyperlink ref="G4" r:id="rId17"/>
+    <hyperlink ref="H4" r:id="rId18"/>
+    <hyperlink ref="G3" r:id="rId19"/>
+    <hyperlink ref="H3" r:id="rId20"/>
+    <hyperlink ref="G25" r:id="rId21"/>
+    <hyperlink ref="H25" r:id="rId22"/>
+    <hyperlink ref="G27" r:id="rId23"/>
+    <hyperlink ref="H27" r:id="rId24"/>
+    <hyperlink ref="G18" r:id="rId25"/>
+    <hyperlink ref="H18" r:id="rId26"/>
+    <hyperlink ref="G14" r:id="rId27"/>
+    <hyperlink ref="H14" r:id="rId28"/>
+    <hyperlink ref="G32" r:id="rId29"/>
+    <hyperlink ref="H32" r:id="rId30"/>
+    <hyperlink ref="G5" r:id="rId31"/>
+    <hyperlink ref="H5" r:id="rId32"/>
+    <hyperlink ref="G16" r:id="rId33"/>
+    <hyperlink ref="H16" r:id="rId34"/>
+    <hyperlink ref="G2" r:id="rId35"/>
+    <hyperlink ref="H2" r:id="rId36"/>
+    <hyperlink ref="G23" r:id="rId37"/>
+    <hyperlink ref="H23" r:id="rId38"/>
+    <hyperlink ref="G12" r:id="rId39"/>
+    <hyperlink ref="H12" r:id="rId40"/>
+    <hyperlink ref="G6" r:id="rId41"/>
+    <hyperlink ref="H6" r:id="rId42"/>
+    <hyperlink ref="G9" r:id="rId43"/>
+    <hyperlink ref="H9" r:id="rId44"/>
+    <hyperlink ref="G24" r:id="rId45"/>
+    <hyperlink ref="H24" r:id="rId46"/>
+    <hyperlink ref="G13" r:id="rId47"/>
+    <hyperlink ref="H13" r:id="rId48"/>
+    <hyperlink ref="G7" r:id="rId49"/>
+    <hyperlink ref="H7" r:id="rId50"/>
+    <hyperlink ref="G30" r:id="rId51"/>
+    <hyperlink ref="H30" r:id="rId52"/>
+    <hyperlink ref="G31" r:id="rId53"/>
+    <hyperlink ref="H31" r:id="rId54"/>
+    <hyperlink ref="G8" r:id="rId55"/>
+    <hyperlink ref="H8" r:id="rId56"/>
+    <hyperlink ref="G28" r:id="rId57"/>
+    <hyperlink ref="H28" r:id="rId58"/>
+    <hyperlink ref="G19" r:id="rId59"/>
+    <hyperlink ref="H19" r:id="rId60"/>
+    <hyperlink ref="G33" r:id="rId61"/>
+    <hyperlink ref="H33" r:id="rId62"/>
+    <hyperlink ref="G11" r:id="rId63"/>
+    <hyperlink ref="H11" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId97"/>
+  <pageSetup orientation="landscape" r:id="rId65"/>
 </worksheet>
 </file>
 
@@ -2676,22 +1844,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>210</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>211</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
@@ -2702,16 +1870,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
@@ -2722,16 +1890,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
@@ -2742,16 +1910,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
@@ -2762,16 +1930,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
@@ -2782,16 +1950,16 @@
         <v>0.5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
@@ -2802,16 +1970,16 @@
         <v>0.5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
@@ -2822,16 +1990,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
@@ -2842,16 +2010,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
@@ -2862,16 +2030,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
@@ -2882,16 +2050,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
@@ -2902,16 +2070,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
@@ -2922,16 +2090,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
@@ -2942,16 +2110,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
@@ -2962,16 +2130,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
@@ -2982,16 +2150,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
@@ -3002,16 +2170,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>220</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
@@ -3022,16 +2190,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>221</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
@@ -3042,16 +2210,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>220</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
@@ -3062,16 +2230,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
@@ -3082,16 +2250,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
@@ -3102,16 +2270,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
@@ -3122,16 +2290,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>221</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
@@ -3142,16 +2310,16 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
@@ -3162,16 +2330,16 @@
         <v>0.5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
@@ -3182,16 +2350,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
@@ -3202,16 +2370,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
@@ -3222,16 +2390,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
@@ -3242,16 +2410,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
@@ -3262,16 +2430,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
@@ -3282,16 +2450,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
@@ -3302,16 +2470,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
@@ -3322,16 +2490,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
@@ -3342,16 +2510,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
@@ -3362,16 +2530,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>222</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
@@ -3382,16 +2550,16 @@
         <v>0.5</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>217</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
@@ -3402,16 +2570,16 @@
         <v>0.5</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>214</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
@@ -3422,16 +2590,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3442,16 +2610,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>167</v>
+        <v>62</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>223</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3462,16 +2630,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3482,16 +2650,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>167</v>
+        <v>62</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>221</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3502,16 +2670,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>183</v>
+        <v>66</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>167</v>
+        <v>62</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>223</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3522,16 +2690,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>178</v>
+        <v>65</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>221</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3542,16 +2710,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3562,16 +2730,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>221</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3582,16 +2750,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3602,16 +2770,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>223</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3622,16 +2790,16 @@
         <v>0.5</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>203</v>
+        <v>70</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>218</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3642,16 +2810,16 @@
         <v>0.5</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>188</v>
+        <v>67</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:6">

</xml_diff>

<commit_message>
:sparkles: feat: update data
</commit_message>
<xml_diff>
--- a/data/DadosCopaDoMundoQatar2022.xlsx
+++ b/data/DadosCopaDoMundoQatar2022.xlsx
@@ -863,7 +863,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -915,13 +915,13 @@
         <v>21</v>
       </c>
       <c r="D2" s="13">
-        <v>88.9</v>
+        <v>90</v>
       </c>
       <c r="E2" s="11">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="F2" s="11">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>126</v>
@@ -941,13 +941,13 @@
         <v>4</v>
       </c>
       <c r="D3" s="13">
-        <v>62</v>
+        <v>60.4</v>
       </c>
       <c r="E3" s="11">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="F3" s="11">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>110</v>
@@ -967,10 +967,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="13">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" s="11">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="F4" s="11">
         <v>0.4</v>
@@ -993,13 +993,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="13">
-        <v>62.4</v>
+        <v>63.1</v>
       </c>
       <c r="E5" s="11">
         <v>1.6</v>
       </c>
       <c r="F5" s="11">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>122</v>
@@ -1019,7 +1019,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="13">
-        <v>79.400000000000006</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="E6" s="11">
         <v>2.4</v>
@@ -1045,13 +1045,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="13">
-        <v>93.5</v>
+        <v>92.9</v>
       </c>
       <c r="E7" s="11">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="11">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>140</v>
@@ -1071,10 +1071,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="13">
-        <v>64.5</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="E8" s="11">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="F8" s="11">
         <v>0.8</v>
@@ -1097,13 +1097,13 @@
         <v>11</v>
       </c>
       <c r="D9" s="13">
-        <v>71.5</v>
+        <v>71.8</v>
       </c>
       <c r="E9" s="11">
         <v>2</v>
       </c>
       <c r="F9" s="11">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>134</v>
@@ -1123,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="13">
-        <v>48.5</v>
+        <v>48.2</v>
       </c>
       <c r="E10" s="11">
         <v>1.4</v>
       </c>
       <c r="F10" s="11">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>92</v>
@@ -1149,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="13">
-        <v>70.3</v>
+        <v>72.7</v>
       </c>
       <c r="E11" s="11">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="F11" s="11">
         <v>0.7</v>
@@ -1175,13 +1175,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="13">
-        <v>52.9</v>
+        <v>52.7</v>
       </c>
       <c r="E12" s="11">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="F12" s="11">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>130</v>
@@ -1201,10 +1201,10 @@
         <v>25</v>
       </c>
       <c r="D13" s="13">
-        <v>80.900000000000006</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="E13" s="11">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F13" s="11">
         <v>0.6</v>
@@ -1227,10 +1227,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="13">
-        <v>77.7</v>
+        <v>76.7</v>
       </c>
       <c r="E14" s="11">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="11">
         <v>0.6</v>
@@ -1253,7 +1253,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="13">
-        <v>75.8</v>
+        <v>73.8</v>
       </c>
       <c r="E15" s="11">
         <v>1.9</v>
@@ -1279,13 +1279,13 @@
         <v>22</v>
       </c>
       <c r="D16" s="13">
-        <v>90.6</v>
+        <v>89.2</v>
       </c>
       <c r="E16" s="11">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="F16" s="11">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>124</v>
@@ -1305,13 +1305,13 @@
         <v>42</v>
       </c>
       <c r="D17" s="13">
-        <v>72.599999999999994</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="E17" s="11">
         <v>1.9</v>
       </c>
       <c r="F17" s="11">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>104</v>
@@ -1331,10 +1331,10 @@
         <v>19</v>
       </c>
       <c r="D18" s="13">
-        <v>90.1</v>
+        <v>88.6</v>
       </c>
       <c r="E18" s="11">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="F18" s="11">
         <v>0.5</v>
@@ -1357,7 +1357,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="13">
-        <v>60.5</v>
+        <v>60.6</v>
       </c>
       <c r="E19" s="11">
         <v>1.6</v>
@@ -1383,13 +1383,13 @@
         <v>23</v>
       </c>
       <c r="D20" s="13">
-        <v>84.4</v>
+        <v>84</v>
       </c>
       <c r="E20" s="11">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="F20" s="11">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>98</v>
@@ -1409,13 +1409,13 @@
         <v>18</v>
       </c>
       <c r="D21" s="13">
-        <v>85.4</v>
+        <v>87</v>
       </c>
       <c r="E21" s="11">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="F21" s="11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>100</v>
@@ -1435,10 +1435,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="13">
-        <v>69.3</v>
+        <v>68.3</v>
       </c>
       <c r="E22" s="11">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="F22" s="11">
         <v>0.7</v>
@@ -1461,13 +1461,13 @@
         <v>1</v>
       </c>
       <c r="D23" s="13">
-        <v>73.7</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="E23" s="11">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="F23" s="11">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>128</v>
@@ -1487,7 +1487,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="13">
-        <v>75</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="E24" s="11">
         <v>1.9</v>
@@ -1513,10 +1513,10 @@
         <v>12</v>
       </c>
       <c r="D25" s="13">
-        <v>72.400000000000006</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="E25" s="11">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="F25" s="11">
         <v>0.6</v>
@@ -1539,10 +1539,10 @@
         <v>30</v>
       </c>
       <c r="D26" s="13">
-        <v>65.2</v>
+        <v>62.5</v>
       </c>
       <c r="E26" s="11">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="F26" s="11">
         <v>0.8</v>
@@ -1565,10 +1565,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="13">
-        <v>69</v>
+        <v>65.8</v>
       </c>
       <c r="E27" s="11">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="F27" s="11">
         <v>0.8</v>
@@ -1591,10 +1591,10 @@
         <v>20</v>
       </c>
       <c r="D28" s="13">
-        <v>87.6</v>
+        <v>85.8</v>
       </c>
       <c r="E28" s="11">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="F28" s="11">
         <v>0.5</v>
@@ -1617,10 +1617,10 @@
         <v>6</v>
       </c>
       <c r="D29" s="13">
-        <v>73</v>
+        <v>75.5</v>
       </c>
       <c r="E29" s="11">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="F29" s="11">
         <v>0.6</v>
@@ -1643,13 +1643,13 @@
         <v>27</v>
       </c>
       <c r="D30" s="13">
-        <v>74.7</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="E30" s="11">
         <v>2.2000000000000002</v>
       </c>
       <c r="F30" s="11">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>142</v>
@@ -1669,10 +1669,10 @@
         <v>29</v>
       </c>
       <c r="D31" s="13">
-        <v>77</v>
+        <v>78.5</v>
       </c>
       <c r="E31" s="11">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F31" s="11">
         <v>0.6</v>
@@ -1695,13 +1695,13 @@
         <v>10</v>
       </c>
       <c r="D32" s="13">
-        <v>65.900000000000006</v>
+        <v>67.8</v>
       </c>
       <c r="E32" s="11">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F32" s="11">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>120</v>
@@ -1721,7 +1721,7 @@
         <v>16</v>
       </c>
       <c r="D33" s="13">
-        <v>79.3</v>
+        <v>79.2</v>
       </c>
       <c r="E33" s="11">
         <v>2.1</v>

</xml_diff>